<commit_message>
Cleaning up formatting, done with density portion
</commit_message>
<xml_diff>
--- a/data/grass_data.xlsx
+++ b/data/grass_data.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JlaMacAir/Documents/r_docs/Model-Selection/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D6550F8C-FD16-A545-AD97-77DFFFDE2900}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{8604618A-4F00-354A-934F-956097B128F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12820" yWindow="960" windowWidth="15600" windowHeight="16540"/>
+    <workbookView xWindow="12820" yWindow="960" windowWidth="15600" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="envr_data (2)" sheetId="2" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -901,11 +901,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K51" sqref="K51"/>
+      <selection activeCell="C80" sqref="C80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2360,17 +2360,597 @@
         <v>30</v>
       </c>
     </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>27</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>50</v>
+      </c>
+      <c r="E51">
+        <v>688</v>
+      </c>
+      <c r="F51">
+        <v>0.1542</v>
+      </c>
+      <c r="G51">
+        <v>13.515000000000001</v>
+      </c>
+      <c r="H51">
+        <v>14.475</v>
+      </c>
+      <c r="I51">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>27</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>51</v>
+      </c>
+      <c r="E52">
+        <v>699</v>
+      </c>
+      <c r="F52">
+        <v>0.1368</v>
+      </c>
+      <c r="G52">
+        <v>22.16</v>
+      </c>
+      <c r="H52">
+        <v>11.74</v>
+      </c>
+      <c r="I52">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
+      <c r="C53">
+        <v>4</v>
+      </c>
+      <c r="D53">
+        <v>52</v>
+      </c>
+      <c r="E53">
+        <v>725</v>
+      </c>
+      <c r="F53">
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="G53">
+        <v>18.88</v>
+      </c>
+      <c r="H53">
+        <v>13.4</v>
+      </c>
+      <c r="I53">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>32</v>
+      </c>
+      <c r="C54">
+        <v>4</v>
+      </c>
+      <c r="D54">
+        <v>53</v>
+      </c>
+      <c r="E54">
+        <v>723</v>
+      </c>
+      <c r="F54">
+        <v>8.3299999999999999E-2</v>
+      </c>
+      <c r="G54">
+        <v>18.079999999999998</v>
+      </c>
+      <c r="H54">
+        <v>8.9</v>
+      </c>
+      <c r="I54">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>19</v>
+      </c>
+      <c r="C55">
+        <v>4</v>
+      </c>
+      <c r="D55">
+        <v>54</v>
+      </c>
+      <c r="E55">
+        <v>708</v>
+      </c>
+      <c r="F55">
+        <v>5.6300000000000003E-2</v>
+      </c>
+      <c r="G55">
+        <v>2.5150000000000001</v>
+      </c>
+      <c r="H55">
+        <v>4.25</v>
+      </c>
+      <c r="I55">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>28</v>
+      </c>
+      <c r="C56">
+        <v>4</v>
+      </c>
+      <c r="D56">
+        <v>55</v>
+      </c>
+      <c r="E56">
+        <v>694</v>
+      </c>
+      <c r="F56">
+        <v>0.14660000000000001</v>
+      </c>
+      <c r="G56">
+        <v>34.26</v>
+      </c>
+      <c r="H56">
+        <v>18.54</v>
+      </c>
+      <c r="I56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>23</v>
+      </c>
+      <c r="C57">
+        <v>4</v>
+      </c>
+      <c r="D57">
+        <v>56</v>
+      </c>
+      <c r="E57">
+        <v>689</v>
+      </c>
+      <c r="F57">
+        <v>0.13830000000000001</v>
+      </c>
+      <c r="G57">
+        <v>14.605</v>
+      </c>
+      <c r="H57">
+        <v>6.3250000000000002</v>
+      </c>
+      <c r="I57">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>17</v>
+      </c>
+      <c r="C58">
+        <v>4</v>
+      </c>
+      <c r="D58">
+        <v>57</v>
+      </c>
+      <c r="E58">
+        <v>683</v>
+      </c>
+      <c r="F58">
+        <v>0.1004</v>
+      </c>
+      <c r="G58">
+        <v>20.695</v>
+      </c>
+      <c r="H58">
+        <v>19.52</v>
+      </c>
+      <c r="I58">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>29</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>58</v>
+      </c>
+      <c r="E59">
+        <v>693</v>
+      </c>
+      <c r="F59">
+        <v>0.13009999999999999</v>
+      </c>
+      <c r="G59">
+        <v>31.65</v>
+      </c>
+      <c r="H59">
+        <v>22.74</v>
+      </c>
+      <c r="I59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
+      <c r="C60">
+        <v>4</v>
+      </c>
+      <c r="D60">
+        <v>59</v>
+      </c>
+      <c r="E60">
+        <v>720</v>
+      </c>
+      <c r="F60">
+        <v>6.5500000000000003E-2</v>
+      </c>
+      <c r="G60">
+        <v>12.685</v>
+      </c>
+      <c r="H60">
+        <v>19.13</v>
+      </c>
+      <c r="I60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>40</v>
+      </c>
+      <c r="C61">
+        <v>4</v>
+      </c>
+      <c r="D61">
+        <v>60</v>
+      </c>
+      <c r="E61">
+        <v>727</v>
+      </c>
+      <c r="F61">
+        <v>9.7299999999999998E-2</v>
+      </c>
+      <c r="G61">
+        <v>13.535</v>
+      </c>
+      <c r="H61">
+        <v>29.945</v>
+      </c>
+      <c r="I61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>7</v>
+      </c>
+      <c r="B62">
+        <v>39</v>
+      </c>
+      <c r="C62">
+        <v>4</v>
+      </c>
+      <c r="D62">
+        <v>61</v>
+      </c>
+      <c r="E62">
+        <v>739</v>
+      </c>
+      <c r="F62">
+        <v>0.251</v>
+      </c>
+      <c r="G62">
+        <v>58.145000000000003</v>
+      </c>
+      <c r="H62">
+        <v>63.045000000000002</v>
+      </c>
+      <c r="I62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>38</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+      <c r="D63">
+        <v>62</v>
+      </c>
+      <c r="E63">
+        <v>715</v>
+      </c>
+      <c r="F63">
+        <v>0.14879999999999999</v>
+      </c>
+      <c r="G63">
+        <v>25.364999999999998</v>
+      </c>
+      <c r="H63">
+        <v>32.880000000000003</v>
+      </c>
+      <c r="I63">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>42</v>
+      </c>
+      <c r="C64">
+        <v>4</v>
+      </c>
+      <c r="D64">
+        <v>63</v>
+      </c>
+      <c r="E64">
+        <v>700</v>
+      </c>
+      <c r="F64">
+        <v>7.9100000000000004E-2</v>
+      </c>
+      <c r="G64">
+        <v>30.26</v>
+      </c>
+      <c r="H64">
+        <v>16.895</v>
+      </c>
+      <c r="I64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>23</v>
+      </c>
+      <c r="C65">
+        <v>4</v>
+      </c>
+      <c r="D65">
+        <v>64</v>
+      </c>
+      <c r="E65">
+        <v>689</v>
+      </c>
+      <c r="F65">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G65">
+        <v>14.93</v>
+      </c>
+      <c r="H65">
+        <v>29.504999999999999</v>
+      </c>
+      <c r="I65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>30</v>
+      </c>
+      <c r="C66">
+        <v>5</v>
+      </c>
+      <c r="D66">
+        <v>65</v>
+      </c>
+      <c r="E66">
+        <v>789</v>
+      </c>
+      <c r="F66">
+        <v>0.2114</v>
+      </c>
+      <c r="G66">
+        <v>34.545000000000002</v>
+      </c>
+      <c r="H66">
+        <v>30.885000000000002</v>
+      </c>
+      <c r="I66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>32</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+      <c r="D67">
+        <v>66</v>
+      </c>
+      <c r="E67">
+        <v>767</v>
+      </c>
+      <c r="F67">
+        <v>0.13930000000000001</v>
+      </c>
+      <c r="G67">
+        <v>8.6349999999999998</v>
+      </c>
+      <c r="H67">
+        <v>2.7549999999999999</v>
+      </c>
+      <c r="I67">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>27</v>
+      </c>
+      <c r="C68">
+        <v>5</v>
+      </c>
+      <c r="D68">
+        <v>67</v>
+      </c>
+      <c r="E68">
+        <v>740</v>
+      </c>
+      <c r="F68">
+        <v>0.1138</v>
+      </c>
+      <c r="G68">
+        <v>44.57</v>
+      </c>
+      <c r="H68">
+        <v>20.55</v>
+      </c>
+      <c r="I68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>29</v>
+      </c>
+      <c r="C69">
+        <v>5</v>
+      </c>
+      <c r="D69">
+        <v>68</v>
+      </c>
+      <c r="E69">
+        <v>729</v>
+      </c>
+      <c r="F69">
+        <v>0.1139</v>
+      </c>
+      <c r="G69">
+        <v>30.74</v>
+      </c>
+      <c r="H69">
+        <v>33.405000000000001</v>
+      </c>
+      <c r="I69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70">
+        <v>31</v>
+      </c>
+      <c r="C70">
+        <v>5</v>
+      </c>
+      <c r="D70">
+        <v>69</v>
+      </c>
+      <c r="E70">
+        <v>725</v>
+      </c>
+      <c r="F70">
+        <v>8.0199999999999994E-2</v>
+      </c>
+      <c r="G70">
+        <v>8.17</v>
+      </c>
+      <c r="H70">
+        <v>13.50333333</v>
+      </c>
+      <c r="I70">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I70" sqref="A1:I70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3826,6 +4406,12 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>4</v>
+      </c>
+      <c r="B51">
+        <v>27</v>
+      </c>
       <c r="C51">
         <v>4</v>
       </c>
@@ -3849,6 +4435,12 @@
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>4</v>
+      </c>
+      <c r="B52">
+        <v>27</v>
+      </c>
       <c r="C52">
         <v>4</v>
       </c>
@@ -3872,6 +4464,12 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>3</v>
+      </c>
+      <c r="B53">
+        <v>22</v>
+      </c>
       <c r="C53">
         <v>4</v>
       </c>
@@ -3895,6 +4493,12 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>6</v>
+      </c>
+      <c r="B54">
+        <v>32</v>
+      </c>
       <c r="C54">
         <v>4</v>
       </c>
@@ -3918,6 +4522,12 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>4</v>
+      </c>
+      <c r="B55">
+        <v>19</v>
+      </c>
       <c r="C55">
         <v>4</v>
       </c>
@@ -3941,6 +4551,12 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>5</v>
+      </c>
+      <c r="B56">
+        <v>28</v>
+      </c>
       <c r="C56">
         <v>4</v>
       </c>
@@ -3964,6 +4580,12 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>4</v>
+      </c>
+      <c r="B57">
+        <v>23</v>
+      </c>
       <c r="C57">
         <v>4</v>
       </c>
@@ -3987,6 +4609,12 @@
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>17</v>
+      </c>
       <c r="C58">
         <v>4</v>
       </c>
@@ -4010,6 +4638,12 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>5</v>
+      </c>
+      <c r="B59">
+        <v>29</v>
+      </c>
       <c r="C59">
         <v>4</v>
       </c>
@@ -4033,6 +4667,12 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>4</v>
+      </c>
+      <c r="B60">
+        <v>26</v>
+      </c>
       <c r="C60">
         <v>4</v>
       </c>
@@ -4056,6 +4696,12 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>6</v>
+      </c>
+      <c r="B61">
+        <v>40</v>
+      </c>
       <c r="C61">
         <v>4</v>
       </c>
@@ -4079,6 +4725,12 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>7</v>
+      </c>
+      <c r="B62">
+        <v>39</v>
+      </c>
       <c r="C62">
         <v>4</v>
       </c>
@@ -4102,6 +4754,12 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>5</v>
+      </c>
+      <c r="B63">
+        <v>38</v>
+      </c>
       <c r="C63">
         <v>4</v>
       </c>
@@ -4125,6 +4783,12 @@
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>4</v>
+      </c>
+      <c r="B64">
+        <v>42</v>
+      </c>
       <c r="C64">
         <v>4</v>
       </c>
@@ -4147,7 +4811,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>23</v>
+      </c>
       <c r="C65">
         <v>4</v>
       </c>
@@ -4170,7 +4840,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>30</v>
+      </c>
       <c r="C66">
         <v>5</v>
       </c>
@@ -4193,7 +4869,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>4</v>
+      </c>
+      <c r="B67">
+        <v>32</v>
+      </c>
       <c r="C67">
         <v>5</v>
       </c>
@@ -4216,7 +4898,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>27</v>
+      </c>
       <c r="C68">
         <v>5</v>
       </c>
@@ -4239,7 +4927,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="69" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>29</v>
+      </c>
       <c r="C69">
         <v>5</v>
       </c>
@@ -4262,7 +4956,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>4</v>
+      </c>
+      <c r="B70">
+        <v>31</v>
+      </c>
       <c r="C70">
         <v>5</v>
       </c>
@@ -4285,7 +4985,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="71" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C71">
         <v>5</v>
       </c>
@@ -4308,7 +5008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C72">
         <v>5</v>
       </c>
@@ -4331,7 +5031,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="73" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C73">
         <v>5</v>
       </c>
@@ -4354,7 +5054,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="74" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C74">
         <v>5</v>
       </c>
@@ -4377,7 +5077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C75">
         <v>5</v>
       </c>
@@ -4400,7 +5100,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C76">
         <v>5</v>
       </c>
@@ -4423,7 +5123,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="77" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C77">
         <v>5</v>
       </c>
@@ -4446,7 +5146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="78" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C78">
         <v>5</v>
       </c>
@@ -4469,7 +5169,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C79">
         <v>5</v>
       </c>
@@ -4492,7 +5192,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="80" spans="3:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C80">
         <v>5</v>
       </c>

</xml_diff>